<commit_message>
Add 4 Stage Registers vhd
</commit_message>
<xml_diff>
--- a/controller.xlsx
+++ b/controller.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="273">
   <si>
     <t>RegDst</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -480,10 +480,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>4-2 sign</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>7-0 zero</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1103,6 +1099,14 @@
   </si>
   <si>
     <t>others</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg1/2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2 zero</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1576,7 +1580,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1608,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I1">
         <v>1</v>
@@ -1649,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>77</v>
@@ -1676,7 +1680,7 @@
         <v>4</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
@@ -1687,40 +1691,40 @@
         <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O3" s="3">
         <v>0</v>
@@ -1737,28 +1741,28 @@
         <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>83</v>
@@ -1787,19 +1791,19 @@
         <v>86</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>97</v>
@@ -1816,7 +1820,7 @@
     </row>
     <row r="6" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>41</v>
@@ -1834,16 +1838,16 @@
         <v>79</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>102</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>97</v>
@@ -1870,28 +1874,28 @@
         <v>61</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>231</v>
-      </c>
       <c r="G7" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>88</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>83</v>
@@ -1921,10 +1925,10 @@
         <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>74</v>
@@ -1936,7 +1940,7 @@
         <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>83</v>
@@ -1962,16 +1966,16 @@
         <v>82</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>80</v>
@@ -2007,16 +2011,16 @@
         <v>82</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>80</v>
@@ -2052,13 +2056,13 @@
         <v>82</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>71</v>
@@ -2100,10 +2104,10 @@
         <v>86</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>71</v>
@@ -2112,10 +2116,10 @@
         <v>44</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>83</v>
@@ -2142,13 +2146,13 @@
         <v>82</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>73</v>
@@ -2175,7 +2179,7 @@
     </row>
     <row r="14" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -2187,16 +2191,16 @@
         <v>82</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>104</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>99</v>
@@ -2232,13 +2236,13 @@
         <v>82</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>71</v>
@@ -2247,7 +2251,7 @@
         <v>80</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>81</v>
@@ -2277,13 +2281,13 @@
         <v>82</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>44</v>
@@ -2322,16 +2326,16 @@
         <v>82</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>80</v>
@@ -2340,7 +2344,7 @@
         <v>90</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>83</v>
@@ -2367,16 +2371,16 @@
         <v>82</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>80</v>
@@ -2412,16 +2416,16 @@
         <v>83</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>80</v>
@@ -2460,13 +2464,13 @@
         <v>104</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>80</v>
@@ -2502,19 +2506,19 @@
         <v>82</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>44</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>90</v>
@@ -2541,25 +2545,25 @@
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>92</v>
@@ -2591,19 +2595,19 @@
         <v>82</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>72</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>93</v>
@@ -2636,19 +2640,19 @@
         <v>82</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>44</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>94</v>
@@ -2681,22 +2685,22 @@
         <v>82</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>73</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>81</v>
@@ -2726,22 +2730,22 @@
         <v>82</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>73</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>81</v>
@@ -2771,22 +2775,22 @@
         <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>81</v>
@@ -2815,13 +2819,13 @@
         <v>82</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>72</v>
@@ -2863,10 +2867,10 @@
         <v>86</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>44</v>
@@ -2905,13 +2909,13 @@
         <v>82</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>73</v>
@@ -2923,7 +2927,7 @@
         <v>91</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L30" s="12" t="s">
         <v>83</v>
@@ -2952,13 +2956,13 @@
         <v>82</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>75</v>
@@ -2997,13 +3001,13 @@
         <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>76</v>
@@ -3107,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3130,18 +3134,18 @@
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="K2" s="8"/>
       <c r="M2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -3157,21 +3161,21 @@
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8">
         <v>0</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K3" s="8"/>
       <c r="N3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
@@ -3189,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8">
@@ -3200,10 +3204,10 @@
       </c>
       <c r="K4" s="8"/>
       <c r="N4" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -3224,10 +3228,10 @@
       <c r="I5" s="8"/>
       <c r="K5" s="8"/>
       <c r="N5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -3238,27 +3242,27 @@
         <v>108</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>115</v>
+        <v>272</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K6" s="8"/>
       <c r="N6" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -3269,27 +3273,27 @@
         <v>109</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="10"/>
@@ -3302,27 +3306,27 @@
         <v>110</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" s="8">
         <v>1000</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="10"/>
@@ -3335,30 +3339,30 @@
         <v>111</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K9" s="8">
         <v>1001</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
@@ -3366,36 +3370,36 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="8">
         <v>1010</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
@@ -3406,59 +3410,62 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" s="8">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>271</v>
       </c>
       <c r="K12" s="8"/>
       <c r="N12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -3469,28 +3476,33 @@
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" s="8"/>
+        <v>153</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>265</v>
+      </c>
       <c r="N13" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
@@ -3501,23 +3513,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="K14" s="8"/>
+        <v>154</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="N14" s="2"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -3532,12 +3549,17 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="K15" s="8"/>
+        <v>191</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1001</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="N15" s="2"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -3550,17 +3572,22 @@
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="K16" s="8"/>
+        <v>194</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1010</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
@@ -3572,22 +3599,27 @@
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9" t="s">
         <v>104</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="K17" s="8"/>
+        <v>171</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1111</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>270</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -3604,13 +3636,13 @@
         <v>106</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H18" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>203</v>
       </c>
       <c r="K18" s="8"/>
       <c r="N18" s="2"/>
@@ -3624,16 +3656,16 @@
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H19" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="9"/>
@@ -3644,22 +3676,22 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H20" s="9">
         <v>1101</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
@@ -3674,14 +3706,14 @@
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -3698,14 +3730,14 @@
         <v>1</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -3722,7 +3754,7 @@
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>44</v>
@@ -3739,16 +3771,16 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -3766,13 +3798,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="8"/>
       <c r="G25" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="8"/>
@@ -3790,10 +3822,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
@@ -3802,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -3818,14 +3850,14 @@
         <v>0</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="9">
         <v>1</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
@@ -3841,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="9"/>
@@ -3857,7 +3889,7 @@
     <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D29" s="8"/>
       <c r="G29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="8"/>
@@ -3873,10 +3905,10 @@
       <c r="D30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -3892,10 +3924,10 @@
       <c r="D31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -3911,10 +3943,10 @@
       <c r="D32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
@@ -3931,10 +3963,10 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>

</xml_diff>

<commit_message>
Fix bugs of ALUOp, ForwardUnit
</commit_message>
<xml_diff>
--- a/controller.xlsx
+++ b/controller.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="277">
   <si>
     <t>RegDst</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -719,10 +719,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>NoOper</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1034,10 +1030,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>(7-0)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>(7-0) 101</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1107,6 +1099,30 @@
   </si>
   <si>
     <t>4-2 zero</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NoOper</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1189,7 +1205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1267,6 +1283,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1579,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1593,7 +1616,8 @@
     <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="11.75" customWidth="1"/>
     <col min="9" max="9" width="11.125" customWidth="1"/>
-    <col min="10" max="11" width="9.625" customWidth="1"/>
+    <col min="10" max="10" width="9.625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="9.625" customWidth="1"/>
     <col min="12" max="13" width="9.25" customWidth="1"/>
     <col min="15" max="15" width="9" style="25"/>
   </cols>
@@ -1612,12 +1636,12 @@
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I1">
         <v>1</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="28">
         <v>4</v>
       </c>
       <c r="K1">
@@ -1659,12 +1683,12 @@
         <v>155</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="29" t="s">
         <v>87</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1691,10 +1715,10 @@
         <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>174</v>
@@ -1706,25 +1730,25 @@
         <v>173</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>175</v>
+      <c r="J3" s="30" t="s">
+        <v>271</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O3" s="3">
         <v>0</v>
@@ -1741,10 +1765,10 @@
         <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>44</v>
@@ -1753,16 +1777,16 @@
         <v>156</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>83</v>
@@ -1791,18 +1815,18 @@
         <v>86</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="29" t="s">
         <v>158</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1820,7 +1844,7 @@
     </row>
     <row r="6" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>41</v>
@@ -1838,15 +1862,15 @@
         <v>79</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="29" t="s">
         <v>170</v>
       </c>
       <c r="K6" s="12" t="s">
@@ -1874,28 +1898,28 @@
         <v>61</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>230</v>
-      </c>
       <c r="G7" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="J7" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" s="29" t="s">
         <v>88</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>83</v>
@@ -1925,10 +1949,10 @@
         <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>74</v>
@@ -1936,7 +1960,7 @@
       <c r="I8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="29" t="s">
         <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1966,21 +1990,21 @@
         <v>82</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K9" s="12" t="s">
@@ -2008,24 +2032,24 @@
         <v>44</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>82</v>
+        <v>236</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K10" s="12" t="s">
@@ -2056,13 +2080,13 @@
         <v>82</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>71</v>
@@ -2070,7 +2094,7 @@
       <c r="I11" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K11" s="12" t="s">
@@ -2104,10 +2128,10 @@
         <v>86</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>71</v>
@@ -2115,8 +2139,8 @@
       <c r="I12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>204</v>
+      <c r="J12" s="29" t="s">
+        <v>203</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>123</v>
@@ -2146,13 +2170,13 @@
         <v>82</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>73</v>
@@ -2160,8 +2184,8 @@
       <c r="I13" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>91</v>
+      <c r="J13" s="29" t="s">
+        <v>273</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>81</v>
@@ -2179,7 +2203,7 @@
     </row>
     <row r="14" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -2191,22 +2215,22 @@
         <v>82</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>104</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>91</v>
+      <c r="J14" s="29" t="s">
+        <v>272</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>81</v>
@@ -2236,13 +2260,13 @@
         <v>82</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>71</v>
@@ -2250,8 +2274,8 @@
       <c r="I15" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>191</v>
+      <c r="J15" s="29" t="s">
+        <v>190</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>81</v>
@@ -2281,13 +2305,13 @@
         <v>82</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>44</v>
@@ -2295,8 +2319,8 @@
       <c r="I16" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>91</v>
+      <c r="J16" s="29" t="s">
+        <v>273</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>81</v>
@@ -2326,25 +2350,25 @@
         <v>82</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>83</v>
@@ -2371,21 +2395,21 @@
         <v>82</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K18" s="12" t="s">
@@ -2416,21 +2440,21 @@
         <v>83</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K19" s="12" t="s">
@@ -2464,18 +2488,18 @@
         <v>104</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K20" s="12" t="s">
@@ -2506,21 +2530,21 @@
         <v>82</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>44</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="J21" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>90</v>
       </c>
       <c r="K21" s="12" t="s">
@@ -2545,19 +2569,19 @@
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>73</v>
@@ -2565,7 +2589,7 @@
       <c r="I22" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="29" t="s">
         <v>92</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -2595,13 +2619,13 @@
         <v>82</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>72</v>
@@ -2609,7 +2633,7 @@
       <c r="I23" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="29" t="s">
         <v>93</v>
       </c>
       <c r="K23" s="12" t="s">
@@ -2640,13 +2664,13 @@
         <v>82</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>44</v>
@@ -2654,7 +2678,7 @@
       <c r="I24" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="29" t="s">
         <v>94</v>
       </c>
       <c r="K24" s="12" t="s">
@@ -2685,13 +2709,13 @@
         <v>82</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>73</v>
@@ -2699,8 +2723,8 @@
       <c r="I25" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>191</v>
+      <c r="J25" s="29" t="s">
+        <v>190</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>81</v>
@@ -2730,13 +2754,13 @@
         <v>82</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>73</v>
@@ -2744,8 +2768,8 @@
       <c r="I26" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>219</v>
+      <c r="J26" s="29" t="s">
+        <v>218</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>81</v>
@@ -2775,13 +2799,13 @@
         <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>73</v>
@@ -2789,8 +2813,8 @@
       <c r="I27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>220</v>
+      <c r="J27" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>81</v>
@@ -2819,13 +2843,13 @@
         <v>82</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>72</v>
@@ -2833,7 +2857,7 @@
       <c r="I28" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="29" t="s">
         <v>33</v>
       </c>
       <c r="K28" s="12" t="s">
@@ -2867,10 +2891,10 @@
         <v>86</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>44</v>
@@ -2878,7 +2902,7 @@
       <c r="I29" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="29" t="s">
         <v>91</v>
       </c>
       <c r="K29" s="12" t="s">
@@ -2909,13 +2933,13 @@
         <v>82</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>73</v>
@@ -2923,7 +2947,7 @@
       <c r="I30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="29" t="s">
         <v>91</v>
       </c>
       <c r="K30" s="12" t="s">
@@ -2956,13 +2980,13 @@
         <v>82</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>75</v>
@@ -2970,8 +2994,8 @@
       <c r="I31" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="23" t="s">
-        <v>91</v>
+      <c r="J31" s="29" t="s">
+        <v>274</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>81</v>
@@ -3001,13 +3025,13 @@
         <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>76</v>
@@ -3015,8 +3039,8 @@
       <c r="I32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>91</v>
+      <c r="J32" s="29" t="s">
+        <v>273</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>81</v>
@@ -3041,7 +3065,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="5"/>
@@ -3057,7 +3081,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="5"/>
@@ -3073,7 +3097,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="29"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="5"/>
@@ -3089,7 +3113,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="29"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="5"/>
@@ -3111,8 +3135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3139,7 +3163,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -3207,7 +3231,7 @@
         <v>166</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -3231,7 +3255,7 @@
         <v>168</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -3242,10 +3266,10 @@
         <v>108</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
@@ -3255,14 +3279,14 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K6" s="8"/>
       <c r="N6" s="2" t="s">
         <v>169</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -3284,16 +3308,16 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="10"/>
@@ -3317,7 +3341,7 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>149</v>
@@ -3326,7 +3350,7 @@
         <v>1000</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="10"/>
@@ -3346,11 +3370,11 @@
         <v>133</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>150</v>
@@ -3359,10 +3383,10 @@
         <v>1001</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
@@ -3384,7 +3408,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>151</v>
@@ -3393,7 +3417,7 @@
         <v>1010</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>165</v>
@@ -3417,7 +3441,7 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>152</v>
@@ -3426,13 +3450,13 @@
         <v>1110</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>166</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
@@ -3452,20 +3476,20 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K12" s="8"/>
       <c r="N12" s="2" t="s">
         <v>168</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -3487,22 +3511,22 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>153</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>169</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
@@ -3524,7 +3548,7 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>154</v>
@@ -3549,10 +3573,10 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K15" s="8">
         <v>1001</v>
@@ -3577,10 +3601,10 @@
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K16" s="8">
         <v>1010</v>
@@ -3609,7 +3633,7 @@
         <v>145</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>171</v>
@@ -3618,7 +3642,7 @@
         <v>1111</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="10"/>
@@ -3636,13 +3660,13 @@
         <v>106</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H18" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="K18" s="8"/>
       <c r="N18" s="2"/>
@@ -3659,13 +3683,13 @@
         <v>133</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H19" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="9"/>
@@ -3691,7 +3715,7 @@
         <v>1101</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
@@ -3715,8 +3739,12 @@
       <c r="F21" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="H21" s="19">
+        <v>1110</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>275</v>
+      </c>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
       <c r="N21" s="2"/>
@@ -3739,8 +3767,12 @@
       <c r="F22" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="19">
+        <v>1111</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>276</v>
+      </c>
       <c r="K22" s="8"/>
       <c r="L22" s="9"/>
       <c r="N22" s="2"/>
@@ -3825,7 +3857,7 @@
         <v>126</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
@@ -3905,7 +3937,7 @@
       <c r="D30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>120</v>
@@ -3924,7 +3956,7 @@
       <c r="D31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>167</v>
@@ -3943,7 +3975,7 @@
       <c r="D32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>170</v>
@@ -3963,7 +3995,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Fix bugs of WriteBack sequence, HarzardDetectionUnit
</commit_message>
<xml_diff>
--- a/controller.xlsx
+++ b/controller.xlsx
@@ -990,10 +990,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>T 010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SP 101</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1123,6 +1119,10 @@
   </si>
   <si>
     <t>OUTPUTB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T 100</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1736,7 +1736,7 @@
         <v>173</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>173</v>
@@ -2080,7 +2080,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>231</v>
@@ -2170,7 +2170,7 @@
         <v>82</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>237</v>
@@ -2185,7 +2185,7 @@
         <v>78</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>81</v>
@@ -2215,7 +2215,7 @@
         <v>82</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>104</v>
@@ -2230,7 +2230,7 @@
         <v>99</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>81</v>
@@ -2260,7 +2260,7 @@
         <v>82</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>243</v>
+        <v>276</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>228</v>
@@ -2308,7 +2308,7 @@
         <v>228</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>234</v>
@@ -2320,7 +2320,7 @@
         <v>78</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>81</v>
@@ -2350,7 +2350,7 @@
         <v>82</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>231</v>
@@ -2359,7 +2359,7 @@
         <v>234</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>80</v>
@@ -2440,13 +2440,13 @@
         <v>83</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>231</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>223</v>
@@ -2491,10 +2491,10 @@
         <v>228</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>80</v>
@@ -2536,7 +2536,7 @@
         <v>228</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>44</v>
@@ -2569,7 +2569,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>82</v>
@@ -2581,7 +2581,7 @@
         <v>228</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>73</v>
@@ -2625,7 +2625,7 @@
         <v>228</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>72</v>
@@ -2670,7 +2670,7 @@
         <v>228</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>44</v>
@@ -2709,13 +2709,13 @@
         <v>82</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>243</v>
+        <v>276</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>228</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>73</v>
@@ -2760,7 +2760,7 @@
         <v>237</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>73</v>
@@ -2799,13 +2799,13 @@
         <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>73</v>
@@ -2894,7 +2894,7 @@
         <v>228</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>44</v>
@@ -2939,7 +2939,7 @@
         <v>104</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>73</v>
@@ -2986,7 +2986,7 @@
         <v>232</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>75</v>
@@ -2995,7 +2995,7 @@
         <v>96</v>
       </c>
       <c r="J31" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>81</v>
@@ -3025,7 +3025,7 @@
         <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>228</v>
@@ -3040,7 +3040,7 @@
         <v>96</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>81</v>
@@ -3136,7 +3136,7 @@
   <dimension ref="A2:Q33"/>
   <sheetViews>
     <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3266,7 +3266,7 @@
         <v>108</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>206</v>
@@ -3279,7 +3279,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K6" s="8"/>
       <c r="N6" s="2" t="s">
@@ -3314,10 +3314,10 @@
         <v>177</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="10"/>
@@ -3350,7 +3350,7 @@
         <v>1000</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="10"/>
@@ -3383,7 +3383,7 @@
         <v>1001</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M9" t="s">
         <v>195</v>
@@ -3417,7 +3417,7 @@
         <v>1010</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>165</v>
@@ -3450,7 +3450,7 @@
         <v>1110</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>166</v>
@@ -3482,7 +3482,7 @@
         <v>176</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K12" s="8"/>
       <c r="N12" s="2" t="s">
@@ -3517,10 +3517,10 @@
         <v>153</v>
       </c>
       <c r="K13" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>169</v>
@@ -3642,7 +3642,7 @@
         <v>1111</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="10"/>
@@ -3743,7 +3743,7 @@
         <v>1110</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
@@ -3771,7 +3771,7 @@
         <v>1111</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="9"/>

</xml_diff>

<commit_message>
Fix bugs of BNEZ/BEQZ/BTEQZ
</commit_message>
<xml_diff>
--- a/controller.xlsx
+++ b/controller.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="278">
   <si>
     <t>RegDst</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1123,6 +1123,10 @@
   </si>
   <si>
     <t>T 100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>imme</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1603,7 +1607,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2497,7 +2501,7 @@
         <v>253</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>80</v>
+        <v>277</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>90</v>

</xml_diff>